<commit_message>
generated main text tables
</commit_message>
<xml_diff>
--- a/Output/Table_T.xlsx
+++ b/Output/Table_T.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="89">
   <si>
     <t>model</t>
   </si>
@@ -38,15 +38,15 @@
     <t>AIC</t>
   </si>
   <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>prob</t>
+  </si>
+  <si>
     <t>ER</t>
   </si>
   <si>
-    <t>prob</t>
-  </si>
-  <si>
-    <t>delta</t>
-  </si>
-  <si>
     <t>deltaAIC</t>
   </si>
   <si>
@@ -161,6 +161,12 @@
     <t>37</t>
   </si>
   <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
     <t>a - net chick</t>
   </si>
   <si>
@@ -215,7 +221,7 @@
     <t>d14_rear_nest_brood_size</t>
   </si>
   <si>
-    <t>16.553</t>
+    <t>16.555</t>
   </si>
   <si>
     <t>-0.063</t>
@@ -224,7 +230,7 @@
     <t>0.479</t>
   </si>
   <si>
-    <t>0.272</t>
+    <t>0.273</t>
   </si>
   <si>
     <t>0.074</t>
@@ -251,25 +257,28 @@
     <t>55%</t>
   </si>
   <si>
-    <t>16.858</t>
-  </si>
-  <si>
-    <t>-0.034</t>
-  </si>
-  <si>
-    <t>0.475</t>
-  </si>
-  <si>
-    <t>0.256</t>
-  </si>
-  <si>
-    <t>0.083</t>
-  </si>
-  <si>
-    <t>28%</t>
-  </si>
-  <si>
-    <t>61%</t>
+    <t>16.918</t>
+  </si>
+  <si>
+    <t>-0.042</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>0.258</t>
+  </si>
+  <si>
+    <t>0.084</t>
+  </si>
+  <si>
+    <t>16%</t>
+  </si>
+  <si>
+    <t>11%</t>
+  </si>
+  <si>
+    <t>52%</t>
   </si>
 </sst>
 </file>
@@ -364,22 +373,22 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F2" t="n">
-        <v>16.304</v>
+        <v>16.308</v>
       </c>
       <c r="G2" t="n">
-        <v>16.8</v>
+        <v>16.795</v>
       </c>
       <c r="H2" t="n">
         <v>2550.0</v>
@@ -390,11 +399,11 @@
       <c r="J2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="K2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L2" t="e">
-        <v>#N/A</v>
+      <c r="K2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1.0</v>
       </c>
       <c r="M2" t="n">
         <v>0.0</v>
@@ -405,16 +414,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F3" t="n">
         <v>-0.074</v>
@@ -446,22 +455,22 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F4" t="n">
-        <v>0.433</v>
+        <v>0.432</v>
       </c>
       <c r="G4" t="n">
-        <v>0.527</v>
+        <v>0.525</v>
       </c>
       <c r="H4" t="e">
         <v>#N/A</v>
@@ -487,22 +496,22 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F5" t="n">
-        <v>0.179</v>
+        <v>0.178</v>
       </c>
       <c r="G5" t="n">
-        <v>0.367</v>
+        <v>0.363</v>
       </c>
       <c r="H5" t="e">
         <v>#N/A</v>
@@ -528,22 +537,22 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.157</v>
+        <v>-0.159</v>
       </c>
       <c r="G6" t="n">
-        <v>0.311</v>
+        <v>0.306</v>
       </c>
       <c r="H6" t="e">
         <v>#N/A</v>
@@ -569,16 +578,16 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F7" t="e">
         <v>#N/A</v>
@@ -610,16 +619,16 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F8" t="e">
         <v>#N/A</v>
@@ -651,16 +660,16 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F9" t="e">
         <v>#N/A</v>
@@ -692,16 +701,16 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F10" t="e">
         <v>#N/A</v>
@@ -733,16 +742,16 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F11" t="e">
         <v>#N/A</v>
@@ -774,16 +783,16 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F12" t="e">
         <v>#N/A</v>
@@ -815,16 +824,16 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F13" t="e">
         <v>#N/A</v>
@@ -856,16 +865,16 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F14" t="e">
         <v>#N/A</v>
@@ -897,40 +906,40 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F15" t="n">
-        <v>16.584</v>
+        <v>16.639</v>
       </c>
       <c r="G15" t="n">
-        <v>17.141</v>
+        <v>17.209</v>
       </c>
       <c r="H15" t="n">
         <v>2550.0</v>
       </c>
       <c r="I15" t="n">
-        <v>4246.426112695946</v>
+        <v>4052.5338803138693</v>
       </c>
       <c r="J15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="K15" t="e">
-        <v>#N/A</v>
+      <c r="K15" t="n">
+        <v>0.0</v>
       </c>
       <c r="L15" t="e">
-        <v>#N/A</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="M15" t="n">
-        <v>252.9509955130975</v>
+        <v>59.05876313102044</v>
       </c>
     </row>
     <row r="16">
@@ -938,22 +947,22 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.047</v>
+        <v>-0.054</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.021</v>
+        <v>-0.03</v>
       </c>
       <c r="H16" t="e">
         <v>#N/A</v>
@@ -979,22 +988,22 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F17" t="n">
-        <v>0.427</v>
+        <v>0.435</v>
       </c>
       <c r="G17" t="n">
-        <v>0.525</v>
+        <v>0.527</v>
       </c>
       <c r="H17" t="e">
         <v>#N/A</v>
@@ -1020,22 +1029,22 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F18" t="n">
-        <v>0.167</v>
+        <v>0.16</v>
       </c>
       <c r="G18" t="n">
-        <v>0.352</v>
+        <v>0.357</v>
       </c>
       <c r="H18" t="e">
         <v>#N/A</v>
@@ -1061,22 +1070,22 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.183</v>
+        <v>-0.165</v>
       </c>
       <c r="G19" t="n">
-        <v>0.337</v>
+        <v>0.34</v>
       </c>
       <c r="H19" t="e">
         <v>#N/A</v>
@@ -1102,16 +1111,16 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F20" t="e">
         <v>#N/A</v>
@@ -1143,16 +1152,16 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
         <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="F21" t="e">
         <v>#N/A</v>
@@ -1184,10 +1193,10 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
         <v>62</v>
@@ -1225,10 +1234,10 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
         <v>63</v>
@@ -1266,16 +1275,16 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
         <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F24" t="e">
         <v>#N/A</v>
@@ -1307,16 +1316,16 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
         <v>65</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F25" t="e">
         <v>#N/A</v>
@@ -1348,28 +1357,28 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" t="n">
-        <v>16.304</v>
-      </c>
-      <c r="G26" t="n">
-        <v>16.8</v>
-      </c>
-      <c r="H26" t="n">
-        <v>2550.0</v>
-      </c>
-      <c r="I26" t="n">
-        <v>3993.475117182849</v>
+        <v>79</v>
+      </c>
+      <c r="F26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I26" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J26" t="e">
         <v>#N/A</v>
@@ -1380,8 +1389,8 @@
       <c r="L26" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M26" t="n">
-        <v>0.0</v>
+      <c r="M26" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="27">
@@ -1389,22 +1398,22 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" t="n">
-        <v>-0.074</v>
-      </c>
-      <c r="G27" t="n">
-        <v>-0.051</v>
+        <v>88</v>
+      </c>
+      <c r="F27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G27" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H27" t="e">
         <v>#N/A</v>
@@ -1430,10 +1439,10 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
         <v>55</v>
@@ -1442,28 +1451,28 @@
         <v>69</v>
       </c>
       <c r="F28" t="n">
-        <v>0.433</v>
+        <v>16.308</v>
       </c>
       <c r="G28" t="n">
-        <v>0.527</v>
-      </c>
-      <c r="H28" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I28" t="e">
-        <v>#N/A</v>
+        <v>16.795</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2550.0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>3993.475117182849</v>
       </c>
       <c r="J28" t="e">
         <v>#N/A</v>
       </c>
-      <c r="K28" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L28" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M28" t="e">
-        <v>#N/A</v>
+      <c r="K28" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="29">
@@ -1471,10 +1480,10 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
         <v>56</v>
@@ -1483,10 +1492,10 @@
         <v>70</v>
       </c>
       <c r="F29" t="n">
-        <v>0.179</v>
+        <v>-0.074</v>
       </c>
       <c r="G29" t="n">
-        <v>0.367</v>
+        <v>-0.051</v>
       </c>
       <c r="H29" t="e">
         <v>#N/A</v>
@@ -1512,10 +1521,10 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
         <v>57</v>
@@ -1524,10 +1533,10 @@
         <v>71</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.157</v>
+        <v>0.432</v>
       </c>
       <c r="G30" t="n">
-        <v>0.311</v>
+        <v>0.525</v>
       </c>
       <c r="H30" t="e">
         <v>#N/A</v>
@@ -1553,10 +1562,10 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D31" t="s">
         <v>58</v>
@@ -1564,11 +1573,11 @@
       <c r="E31" t="s">
         <v>72</v>
       </c>
-      <c r="F31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G31" t="e">
-        <v>#N/A</v>
+      <c r="F31" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.363</v>
       </c>
       <c r="H31" t="e">
         <v>#N/A</v>
@@ -1594,10 +1603,10 @@
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
         <v>59</v>
@@ -1605,11 +1614,11 @@
       <c r="E32" t="s">
         <v>73</v>
       </c>
-      <c r="F32" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G32" t="e">
-        <v>#N/A</v>
+      <c r="F32" t="n">
+        <v>-0.159</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.306</v>
       </c>
       <c r="H32" t="e">
         <v>#N/A</v>
@@ -1635,16 +1644,16 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
         <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F33" t="e">
         <v>#N/A</v>
@@ -1676,16 +1685,16 @@
         <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
         <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F34" t="e">
         <v>#N/A</v>
@@ -1717,16 +1726,16 @@
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
         <v>62</v>
       </c>
       <c r="E35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F35" t="e">
         <v>#N/A</v>
@@ -1758,10 +1767,10 @@
         <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
         <v>63</v>
@@ -1799,10 +1808,10 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
         <v>64</v>
@@ -1840,10 +1849,10 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
         <v>65</v>
@@ -1873,6 +1882,88 @@
         <v>#N/A</v>
       </c>
       <c r="M38" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M39" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M40" t="e">
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>